<commit_message>
Adding Validation to ViewModel
</commit_message>
<xml_diff>
--- a/BTS.Web/Sample File/Import BTS Certificate Sample.xlsx
+++ b/BTS.Web/Sample File/Import BTS Certificate Sample.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="151">
   <si>
     <t>No</t>
   </si>
@@ -486,9 +486,6 @@
   </si>
   <si>
     <t>34,5/ 34,5/ 34,5;34,5/ 34,5/ 34,5</t>
-  </si>
-  <si>
-    <t>10,759444</t>
   </si>
   <si>
     <t>VNMOBILE;VNMOBILE</t>
@@ -3159,7 +3156,7 @@
   <dimension ref="A1:J406"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75"/>
@@ -3217,8 +3214,8 @@
       <c r="E2" s="33">
         <v>106.69888899999999</v>
       </c>
-      <c r="F2" t="s">
-        <v>150</v>
+      <c r="F2">
+        <v>10.759444</v>
       </c>
       <c r="G2">
         <v>1</v>
@@ -3240,8 +3237,8 @@
       <c r="E3" s="33">
         <v>106.6932</v>
       </c>
-      <c r="F3" t="s">
-        <v>126</v>
+      <c r="F3">
+        <v>10.772119999999999</v>
       </c>
       <c r="G3">
         <v>1</v>
@@ -3263,8 +3260,8 @@
       <c r="E4" s="33">
         <v>106.68680999999999</v>
       </c>
-      <c r="F4" t="s">
-        <v>134</v>
+      <c r="F4">
+        <v>10.76398</v>
       </c>
       <c r="G4">
         <v>1</v>
@@ -3286,8 +3283,8 @@
       <c r="E5" s="33">
         <v>106.702</v>
       </c>
-      <c r="F5" t="s">
-        <v>143</v>
+      <c r="F5">
+        <v>10.777200000000001</v>
       </c>
       <c r="G5">
         <v>1</v>
@@ -5116,7 +5113,7 @@
         <v>119</v>
       </c>
       <c r="P2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="Q2" t="s">
         <v>120</v>
@@ -5197,7 +5194,7 @@
         <v>129</v>
       </c>
       <c r="P3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="Q3" t="s">
         <v>120</v>
@@ -5278,7 +5275,7 @@
         <v>137</v>
       </c>
       <c r="P4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="Q4" t="s">
         <v>120</v>
@@ -5359,7 +5356,7 @@
         <v>146</v>
       </c>
       <c r="P5" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="Q5" t="s">
         <v>120</v>

</xml_diff>